<commit_message>
Update of benchmark files to 42m depth
</commit_message>
<xml_diff>
--- a/Plaxisfiles/benchmark/Structural Forces D_10.xlsx
+++ b/Plaxisfiles/benchmark/Structural Forces D_10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FKMV\Desktop\COPCAT_branch\COPCATPlaxis\Plaxisfiles\Loc_69L\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Other computers\My Laptop\work1\004 EW\Cospin - EW1\output\loc69_L_42m\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119140F7-F44C-4F86-AE1E-7D5E0B425D04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454FF837-DA6C-491C-ADDE-1D5EFE63C305}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="N" sheetId="1" r:id="rId1"/>
@@ -153,10 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -214,7 +213,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -237,7 +236,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -315,7 +326,7 @@
                   <c:v>0.70509999999999995</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.97</c:v>
+                  <c:v>0.97137878821043999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -396,7 +407,7 @@
                   <c:v>3715148.1882164301</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4217373.9109924799</c:v>
+                  <c:v>4235495.0943433102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -474,7 +485,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251832528"/>
@@ -536,7 +547,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251831216"/>
@@ -584,7 +595,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -635,7 +646,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -646,17 +657,8 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -667,124 +669,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>4217373.9109924799</c:v>
+                  <c:v>4235495.0943433102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4284449.2636098899</c:v>
+                  <c:v>4302531.5954806898</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4421599.4183441196</c:v>
+                  <c:v>4431703.8613596996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4519056.9895853</c:v>
+                  <c:v>4518146.7430723496</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4628946.88624423</c:v>
+                  <c:v>4609100.6883866601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4696886.1091856798</c:v>
+                  <c:v>4665281.3549855398</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4776059.0270261997</c:v>
+                  <c:v>4726903.4452141803</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4846194.9861611901</c:v>
+                  <c:v>4771821.4116742099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4905120.4762008404</c:v>
+                  <c:v>4802094.1402403703</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4951334.1403214801</c:v>
+                  <c:v>4816792.1221114304</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4982005.5781040499</c:v>
+                  <c:v>4806109.4324945798</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4994468.5386776701</c:v>
+                  <c:v>4774892.8022672301</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4987046.6483135698</c:v>
+                  <c:v>4723250.45555415</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4962310.0705819</c:v>
+                  <c:v>4659603.6737921899</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4910076.7461911803</c:v>
+                  <c:v>4580300.7417479204</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4844901.1359844003</c:v>
+                  <c:v>4493880.68601075</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4762292.2830301197</c:v>
+                  <c:v>4393876.3332722997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4662094.1879299898</c:v>
+                  <c:v>4280549.4716282701</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4544288.5230725901</c:v>
+                  <c:v>4154232.72484947</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4408990.8728272496</c:v>
+                  <c:v>4015330.3491565902</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4256449.2996079</c:v>
+                  <c:v>3864320.3109772499</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4087045.3201342402</c:v>
+                  <c:v>3701758.0153174498</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3901297.6409672499</c:v>
+                  <c:v>3528282.2662337301</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3699869.3650770299</c:v>
+                  <c:v>3344624.4091634098</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3483579.9670185</c:v>
+                  <c:v>3151622.2879163302</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3253386.1207580301</c:v>
+                  <c:v>2950279.90771541</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3011313.6971360999</c:v>
+                  <c:v>2754176.8195004999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2758582.54667213</c:v>
+                  <c:v>2548434.0323502799</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2359675.5848610601</c:v>
+                  <c:v>2222280.2424821099</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1945610.4228588899</c:v>
+                  <c:v>1880350.08042416</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1678145.2904486</c:v>
+                  <c:v>1655326.2998215</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1423479.1098921499</c:v>
+                  <c:v>1439695.9809106099</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1183807.7017788701</c:v>
+                  <c:v>1236072.69115966</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>960857.68070996902</c:v>
+                  <c:v>1046432.2915539501</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>661055.73924759496</c:v>
+                  <c:v>791654.05305870902</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>406902.151588879</c:v>
+                  <c:v>577549.35503062897</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>251523.46016816</c:v>
+                  <c:v>448457.15194733901</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>149023.05007300799</c:v>
+                  <c:v>329597.57901366398</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>64601.459795608498</c:v>
+                  <c:v>214205.782486921</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.3596007103389799E-7</c:v>
+                  <c:v>41084.886777708198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -913,7 +915,7 @@
                   <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-41.9</c:v>
+                  <c:v>-42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,7 +923,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D5CB-4D33-B7C8-32007ED442F7}"/>
+              <c16:uniqueId val="{00000003-DDFF-469D-8349-6A22D5896C2F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -991,7 +993,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="621716856"/>
@@ -1053,47 +1055,19 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="621709968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -1101,7 +1075,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1152,7 +1126,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1253,7 +1227,7 @@
                   <c:v>0.70509999999999995</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.97</c:v>
+                  <c:v>0.97137878821043999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1265,76 +1239,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="24"/>
                 <c:pt idx="0">
-                  <c:v>587.76379147609202</c:v>
+                  <c:v>769.59517941906802</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>894.53524404475399</c:v>
+                  <c:v>1095.93721645449</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1685.9540334445801</c:v>
+                  <c:v>1847.6450571768901</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2685.7260619399099</c:v>
+                  <c:v>2702.4626494673798</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3496.8083549493899</c:v>
+                  <c:v>3548.33191101282</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4364.7422105529904</c:v>
+                  <c:v>4389.2933019460697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5199.3908910112796</c:v>
+                  <c:v>5231.4400487534604</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6052.4248793276702</c:v>
+                  <c:v>6072.9728815016297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7156.6485368989897</c:v>
+                  <c:v>7185.4974858649903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7715.98666897149</c:v>
+                  <c:v>7733.8088536306104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8782.8961653280094</c:v>
+                  <c:v>8809.2383050809494</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10339.911103843</c:v>
+                  <c:v>10360.316923390599</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12283.889776092799</c:v>
+                  <c:v>12309.539898790201</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14114.863424078299</c:v>
+                  <c:v>14139.570367816201</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15421.436610549301</c:v>
+                  <c:v>15453.968792120701</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18728.348037871299</c:v>
+                  <c:v>18765.617483101301</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21441.2179917748</c:v>
+                  <c:v>21485.3084719656</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>26502.907300478098</c:v>
+                  <c:v>26564.410371239199</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>31331.188571848899</c:v>
+                  <c:v>31417.981095376301</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35824.977101111399</c:v>
+                  <c:v>35935.318912369003</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>39260.830775698298</c:v>
+                  <c:v>39394.046467443899</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42536.195150443797</c:v>
+                  <c:v>42691.882795442398</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>45465.994903146697</c:v>
+                  <c:v>45640.202475418002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>51612.234836290998</c:v>
+                  <c:v>51859.980828608699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1412,7 +1386,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251832528"/>
@@ -1474,7 +1448,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251831216"/>
@@ -1522,7 +1496,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1573,7 +1547,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="da-DK"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1605,124 +1579,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
                 <c:pt idx="0">
-                  <c:v>0.97</c:v>
+                  <c:v>0.97137878821043999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.94073927832429804</c:v>
+                  <c:v>0.94225836884681102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88135446667655803</c:v>
+                  <c:v>0.88281559108219199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.83829454250995294</c:v>
+                  <c:v>0.83970298389717202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78766515902544598</c:v>
+                  <c:v>0.78903594666788202</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75456720487645301</c:v>
+                  <c:v>0.75590383794708604</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.71391665141795002</c:v>
+                  <c:v>0.71522760791612905</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67419039778418799</c:v>
+                  <c:v>0.67547279103295099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63536301298841302</c:v>
+                  <c:v>0.63662037055786103</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.59744788705166096</c:v>
+                  <c:v>0.59868381165102602</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.56054153920421901</c:v>
+                  <c:v>0.56175781540432501</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.52459239970265004</c:v>
+                  <c:v>0.52579293131129301</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.48959432276173498</c:v>
+                  <c:v>0.49078310014256099</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.45888368651975298</c:v>
+                  <c:v>0.46007268871467599</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.42221758354362099</c:v>
+                  <c:v>0.42339478756267102</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.38977176282044201</c:v>
+                  <c:v>0.39094909728395</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.35816871814615298</c:v>
+                  <c:v>0.35935094724759797</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.32738993751137402</c:v>
+                  <c:v>0.32858186557054098</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.29741413600727401</c:v>
+                  <c:v>0.29862059483989201</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.26821730144302602</c:v>
+                  <c:v>0.26944313833681299</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.23977273954965</c:v>
+                  <c:v>0.241022806027475</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.21205111565814799</c:v>
+                  <c:v>0.213330257275611</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.18502048802422999</c:v>
+                  <c:v>0.18633353556508001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.15864632487983199</c:v>
+                  <c:v>0.15999808752458899</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.132891491385599</c:v>
+                  <c:v>0.13428675283887301</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.10771618046411199</c:v>
+                  <c:v>0.109159699886867</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8.29736055565133E-2</c:v>
+                  <c:v>8.4463989575823503E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.8757636784181298E-2</c:v>
+                  <c:v>6.0299702101401301E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.33425078470871E-2</c:v>
+                  <c:v>2.4973141860952099E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-1.11403354297211E-2</c:v>
+                  <c:v>-9.4079675965762308E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-3.3780880624724299E-2</c:v>
+                  <c:v>-3.1968653732251398E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-5.6247345389732702E-2</c:v>
+                  <c:v>-5.4349178650244599E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-7.8597189355710806E-2</c:v>
+                  <c:v>-7.66082553770535E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.100880590735083</c:v>
+                  <c:v>-9.8796770034495898E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.1342794233274</c:v>
+                  <c:v>-0.13204635856904601</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.16776725085724301</c:v>
+                  <c:v>-0.16537917004389599</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.192448809280408</c:v>
+                  <c:v>-0.18994441555804401</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.21245768606427701</c:v>
+                  <c:v>-0.20985740725969901</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.23479488980530799</c:v>
+                  <c:v>-0.232086793753283</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.27765554575005102</c:v>
+                  <c:v>-0.27699562167408698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1851,7 +1825,7 @@
                   <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-41.9</c:v>
+                  <c:v>-42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1929,7 +1903,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251832528"/>
@@ -1991,7 +1965,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="251831216"/>
@@ -2039,7 +2013,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="da-DK"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2131,46 +2105,6 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3758,522 +3692,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4316,16 +3734,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4755,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4766,76 +4184,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>587.76379147609202</v>
+        <v>769.59517941906802</v>
       </c>
       <c r="C1" s="1">
-        <v>894.53524404475399</v>
+        <v>1095.93721645449</v>
       </c>
       <c r="D1" s="1">
-        <v>1685.9540334445801</v>
+        <v>1847.6450571768901</v>
       </c>
       <c r="E1" s="1">
-        <v>2685.7260619399099</v>
+        <v>2702.4626494673798</v>
       </c>
       <c r="F1" s="1">
-        <v>3496.8083549493899</v>
+        <v>3548.33191101282</v>
       </c>
       <c r="G1" s="1">
-        <v>4364.7422105529904</v>
+        <v>4389.2933019460697</v>
       </c>
       <c r="H1" s="1">
-        <v>5199.3908910112796</v>
+        <v>5231.4400487534604</v>
       </c>
       <c r="I1" s="1">
-        <v>6052.4248793276702</v>
+        <v>6072.9728815016297</v>
       </c>
       <c r="J1" s="1">
-        <v>7156.6485368989897</v>
+        <v>7185.4974858649903</v>
       </c>
       <c r="K1" s="1">
-        <v>7715.98666897149</v>
+        <v>7733.8088536306104</v>
       </c>
       <c r="L1" s="1">
-        <v>8782.8961653280094</v>
+        <v>8809.2383050809494</v>
       </c>
       <c r="M1" s="1">
-        <v>10339.911103843</v>
+        <v>10360.316923390599</v>
       </c>
       <c r="N1" s="1">
-        <v>12283.889776092799</v>
+        <v>12309.539898790201</v>
       </c>
       <c r="O1" s="1">
-        <v>14114.863424078299</v>
+        <v>14139.570367816201</v>
       </c>
       <c r="P1" s="1">
-        <v>15421.436610549301</v>
+        <v>15453.968792120701</v>
       </c>
       <c r="Q1" s="1">
-        <v>18728.348037871299</v>
+        <v>18765.617483101301</v>
       </c>
       <c r="R1" s="1">
-        <v>21441.2179917748</v>
+        <v>21485.3084719656</v>
       </c>
       <c r="S1" s="1">
-        <v>26502.907300478098</v>
+        <v>26564.410371239199</v>
       </c>
       <c r="T1" s="1">
-        <v>31331.188571848899</v>
+        <v>31417.981095376301</v>
       </c>
       <c r="U1" s="1">
-        <v>35824.977101111399</v>
+        <v>35935.318912369003</v>
       </c>
       <c r="V1" s="1">
-        <v>39260.830775698298</v>
+        <v>39394.046467443899</v>
       </c>
       <c r="W1" s="1">
-        <v>42536.195150443797</v>
+        <v>42691.882795442398</v>
       </c>
       <c r="X1" s="1">
-        <v>45465.994903146697</v>
+        <v>45640.202475418002</v>
       </c>
       <c r="Y1" s="1">
-        <v>51612.234836290998</v>
+        <v>51859.980828608699</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -4916,7 +4334,7 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>0</v>
       </c>
       <c r="B4">
@@ -4993,7 +4411,7 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>-0.65</v>
       </c>
       <c r="B5">
@@ -5070,7 +4488,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>-2</v>
       </c>
       <c r="B6">
@@ -5147,7 +4565,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>-3</v>
       </c>
       <c r="B7">
@@ -5224,7 +4642,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>-4.2</v>
       </c>
       <c r="B8">
@@ -5301,7 +4719,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>-5</v>
       </c>
       <c r="B9">
@@ -5378,7 +4796,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>-6</v>
       </c>
       <c r="B10">
@@ -5455,7 +4873,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>-7</v>
       </c>
       <c r="B11">
@@ -5532,7 +4950,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>-8</v>
       </c>
       <c r="B12">
@@ -5609,7 +5027,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>-9</v>
       </c>
       <c r="B13">
@@ -5686,7 +5104,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>-10</v>
       </c>
       <c r="B14">
@@ -5763,7 +5181,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>-11</v>
       </c>
       <c r="B15">
@@ -5840,7 +5258,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>-12</v>
       </c>
       <c r="B16">
@@ -5917,7 +5335,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>-12.9</v>
       </c>
       <c r="B17">
@@ -5994,7 +5412,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>-14</v>
       </c>
       <c r="B18">
@@ -6071,7 +5489,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>-15</v>
       </c>
       <c r="B19">
@@ -6148,7 +5566,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>-16</v>
       </c>
       <c r="B20">
@@ -6225,7 +5643,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>-17</v>
       </c>
       <c r="B21">
@@ -6302,7 +5720,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>-18</v>
       </c>
       <c r="B22">
@@ -6379,7 +5797,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>-19</v>
       </c>
       <c r="B23">
@@ -6456,7 +5874,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>-20</v>
       </c>
       <c r="B24">
@@ -6533,7 +5951,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>-21</v>
       </c>
       <c r="B25">
@@ -6610,7 +6028,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>-22</v>
       </c>
       <c r="B26">
@@ -6687,7 +6105,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>-23</v>
       </c>
       <c r="B27">
@@ -6764,7 +6182,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>-24</v>
       </c>
       <c r="B28">
@@ -6841,7 +6259,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>-25</v>
       </c>
       <c r="B29">
@@ -6918,7 +6336,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>-26</v>
       </c>
       <c r="B30">
@@ -6995,7 +6413,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>-27</v>
       </c>
       <c r="B31">
@@ -7072,7 +6490,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>-28.5</v>
       </c>
       <c r="B32">
@@ -7149,7 +6567,7 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>-30</v>
       </c>
       <c r="B33">
@@ -7226,7 +6644,7 @@
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>-31</v>
       </c>
       <c r="B34">
@@ -7303,7 +6721,7 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>-32</v>
       </c>
       <c r="B35">
@@ -7380,7 +6798,7 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>-33</v>
       </c>
       <c r="B36">
@@ -7457,7 +6875,7 @@
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>-34</v>
       </c>
       <c r="B37">
@@ -7534,7 +6952,7 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>-35.5</v>
       </c>
       <c r="B38">
@@ -7611,7 +7029,7 @@
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>-37</v>
       </c>
       <c r="B39">
@@ -7688,7 +7106,7 @@
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>-38.1</v>
       </c>
       <c r="B40">
@@ -7765,7 +7183,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>-39</v>
       </c>
       <c r="B41">
@@ -7842,7 +7260,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>-40</v>
       </c>
       <c r="B42">
@@ -7919,8 +7337,8 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>-41</v>
+      <c r="A43" s="1">
+        <v>-42</v>
       </c>
       <c r="B43">
         <v>-41598.618631481957</v>
@@ -8005,7 +7423,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8015,76 +7433,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>587.76379147609202</v>
+        <v>769.59517941906802</v>
       </c>
       <c r="C1" s="1">
-        <v>894.53524404475399</v>
+        <v>1095.93721645449</v>
       </c>
       <c r="D1" s="1">
-        <v>1685.9540334445801</v>
+        <v>1847.6450571768901</v>
       </c>
       <c r="E1" s="1">
-        <v>2685.7260619399099</v>
+        <v>2702.4626494673798</v>
       </c>
       <c r="F1" s="1">
-        <v>3496.8083549493899</v>
+        <v>3548.33191101282</v>
       </c>
       <c r="G1" s="1">
-        <v>4364.7422105529904</v>
+        <v>4389.2933019460697</v>
       </c>
       <c r="H1" s="1">
-        <v>5199.3908910112796</v>
+        <v>5231.4400487534604</v>
       </c>
       <c r="I1" s="1">
-        <v>6052.4248793276702</v>
+        <v>6072.9728815016297</v>
       </c>
       <c r="J1" s="1">
-        <v>7156.6485368989897</v>
+        <v>7185.4974858649903</v>
       </c>
       <c r="K1" s="1">
-        <v>7715.98666897149</v>
+        <v>7733.8088536306104</v>
       </c>
       <c r="L1" s="1">
-        <v>8782.8961653280094</v>
+        <v>8809.2383050809494</v>
       </c>
       <c r="M1" s="1">
-        <v>10339.911103843</v>
+        <v>10360.316923390599</v>
       </c>
       <c r="N1" s="1">
-        <v>12283.889776092799</v>
+        <v>12309.539898790201</v>
       </c>
       <c r="O1" s="1">
-        <v>14114.863424078299</v>
+        <v>14139.570367816201</v>
       </c>
       <c r="P1" s="1">
-        <v>15421.436610549301</v>
+        <v>15453.968792120701</v>
       </c>
       <c r="Q1" s="1">
-        <v>18728.348037871299</v>
+        <v>18765.617483101301</v>
       </c>
       <c r="R1" s="1">
-        <v>21441.2179917748</v>
+        <v>21485.3084719656</v>
       </c>
       <c r="S1" s="1">
-        <v>26502.907300478098</v>
+        <v>26564.410371239199</v>
       </c>
       <c r="T1" s="1">
-        <v>31331.188571848899</v>
+        <v>31417.981095376301</v>
       </c>
       <c r="U1" s="1">
-        <v>35824.977101111399</v>
+        <v>35935.318912369003</v>
       </c>
       <c r="V1" s="1">
-        <v>39260.830775698298</v>
+        <v>39394.046467443899</v>
       </c>
       <c r="W1" s="1">
-        <v>42536.195150443797</v>
+        <v>42691.882795442398</v>
       </c>
       <c r="X1" s="1">
-        <v>45465.994903146697</v>
+        <v>45640.202475418002</v>
       </c>
       <c r="Y1" s="1">
-        <v>51612.234836290998</v>
+        <v>51859.980828608699</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8165,108 +7583,108 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>0</v>
       </c>
-      <c r="B4">
-        <f>B1*-2</f>
-        <v>-1175.527582952184</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:Y4" si="0">C1*-2</f>
-        <v>-1789.070488089508</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="1">
+        <f>B1</f>
+        <v>769.59517941906802</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:Y4" si="0">C1</f>
+        <v>1095.93721645449</v>
+      </c>
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>-3371.9080668891602</v>
-      </c>
-      <c r="E4">
+        <v>1847.6450571768901</v>
+      </c>
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>-5371.4521238798197</v>
-      </c>
-      <c r="F4">
+        <v>2702.4626494673798</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>-6993.6167098987798</v>
-      </c>
-      <c r="G4">
+        <v>3548.33191101282</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>-8729.4844211059808</v>
-      </c>
-      <c r="H4">
+        <v>4389.2933019460697</v>
+      </c>
+      <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>-10398.781782022559</v>
-      </c>
-      <c r="I4">
+        <v>5231.4400487534604</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>-12104.84975865534</v>
-      </c>
-      <c r="J4">
+        <v>6072.9728815016297</v>
+      </c>
+      <c r="J4" s="1">
         <f t="shared" si="0"/>
-        <v>-14313.297073797979</v>
-      </c>
-      <c r="K4">
+        <v>7185.4974858649903</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="0"/>
-        <v>-15431.97333794298</v>
-      </c>
-      <c r="L4">
+        <v>7733.8088536306104</v>
+      </c>
+      <c r="L4" s="1">
         <f t="shared" si="0"/>
-        <v>-17565.792330656019</v>
-      </c>
-      <c r="M4">
+        <v>8809.2383050809494</v>
+      </c>
+      <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>-20679.822207686</v>
-      </c>
-      <c r="N4">
+        <v>10360.316923390599</v>
+      </c>
+      <c r="N4" s="1">
         <f t="shared" si="0"/>
-        <v>-24567.779552185599</v>
-      </c>
-      <c r="O4">
+        <v>12309.539898790201</v>
+      </c>
+      <c r="O4" s="1">
         <f t="shared" si="0"/>
-        <v>-28229.726848156599</v>
-      </c>
-      <c r="P4">
+        <v>14139.570367816201</v>
+      </c>
+      <c r="P4" s="1">
         <f t="shared" si="0"/>
-        <v>-30842.873221098602</v>
-      </c>
-      <c r="Q4">
+        <v>15453.968792120701</v>
+      </c>
+      <c r="Q4" s="1">
         <f t="shared" si="0"/>
-        <v>-37456.696075742599</v>
-      </c>
-      <c r="R4">
+        <v>18765.617483101301</v>
+      </c>
+      <c r="R4" s="1">
         <f t="shared" si="0"/>
-        <v>-42882.4359835496</v>
-      </c>
-      <c r="S4">
+        <v>21485.3084719656</v>
+      </c>
+      <c r="S4" s="1">
         <f t="shared" si="0"/>
-        <v>-53005.814600956197</v>
-      </c>
-      <c r="T4">
+        <v>26564.410371239199</v>
+      </c>
+      <c r="T4" s="1">
         <f t="shared" si="0"/>
-        <v>-62662.377143697799</v>
-      </c>
-      <c r="U4">
+        <v>31417.981095376301</v>
+      </c>
+      <c r="U4" s="1">
         <f t="shared" si="0"/>
-        <v>-71649.954202222798</v>
-      </c>
-      <c r="V4">
+        <v>35935.318912369003</v>
+      </c>
+      <c r="V4" s="1">
         <f t="shared" si="0"/>
-        <v>-78521.661551396595</v>
-      </c>
-      <c r="W4">
+        <v>39394.046467443899</v>
+      </c>
+      <c r="W4" s="1">
         <f t="shared" si="0"/>
-        <v>-85072.390300887593</v>
-      </c>
-      <c r="X4">
+        <v>42691.882795442398</v>
+      </c>
+      <c r="X4" s="1">
         <f t="shared" si="0"/>
-        <v>-90931.989806293393</v>
-      </c>
-      <c r="Y4">
+        <v>45640.202475418002</v>
+      </c>
+      <c r="Y4" s="1">
         <f t="shared" si="0"/>
-        <v>-103224.469672582</v>
+        <v>51859.980828608699</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>-0.65</v>
       </c>
       <c r="B5">
@@ -8343,7 +7761,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>-2</v>
       </c>
       <c r="B6">
@@ -8420,7 +7838,7 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>-3</v>
       </c>
       <c r="B7">
@@ -8497,7 +7915,7 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>-4.2</v>
       </c>
       <c r="B8">
@@ -8574,7 +7992,7 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>-5</v>
       </c>
       <c r="B9">
@@ -8651,7 +8069,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>-6</v>
       </c>
       <c r="B10">
@@ -8728,7 +8146,7 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>-7</v>
       </c>
       <c r="B11">
@@ -8805,7 +8223,7 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>-8</v>
       </c>
       <c r="B12">
@@ -8882,7 +8300,7 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>-9</v>
       </c>
       <c r="B13">
@@ -8959,7 +8377,7 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>-10</v>
       </c>
       <c r="B14">
@@ -9036,7 +8454,7 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>-11</v>
       </c>
       <c r="B15">
@@ -9113,7 +8531,7 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>-12</v>
       </c>
       <c r="B16">
@@ -9190,7 +8608,7 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>-12.9</v>
       </c>
       <c r="B17">
@@ -9267,7 +8685,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>-14</v>
       </c>
       <c r="B18">
@@ -9344,7 +8762,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>-15</v>
       </c>
       <c r="B19">
@@ -9421,7 +8839,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>-16</v>
       </c>
       <c r="B20">
@@ -9498,7 +8916,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>-17</v>
       </c>
       <c r="B21">
@@ -9575,7 +8993,7 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>-18</v>
       </c>
       <c r="B22">
@@ -9652,7 +9070,7 @@
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>-19</v>
       </c>
       <c r="B23">
@@ -9729,7 +9147,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>-20</v>
       </c>
       <c r="B24">
@@ -9806,7 +9224,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>-21</v>
       </c>
       <c r="B25">
@@ -9883,7 +9301,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>-22</v>
       </c>
       <c r="B26">
@@ -9960,7 +9378,7 @@
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>-23</v>
       </c>
       <c r="B27">
@@ -10037,7 +9455,7 @@
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>-24</v>
       </c>
       <c r="B28">
@@ -10114,7 +9532,7 @@
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>-25</v>
       </c>
       <c r="B29">
@@ -10191,7 +9609,7 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>-26</v>
       </c>
       <c r="B30">
@@ -10268,7 +9686,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>-27</v>
       </c>
       <c r="B31">
@@ -10345,7 +9763,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="1">
         <v>-28.5</v>
       </c>
       <c r="B32">
@@ -10422,7 +9840,7 @@
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="1">
         <v>-30</v>
       </c>
       <c r="B33">
@@ -10499,7 +9917,7 @@
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="1">
         <v>-31</v>
       </c>
       <c r="B34">
@@ -10576,7 +9994,7 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="1">
         <v>-32</v>
       </c>
       <c r="B35">
@@ -10653,7 +10071,7 @@
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="1">
         <v>-33</v>
       </c>
       <c r="B36">
@@ -10730,7 +10148,7 @@
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="1">
         <v>-34</v>
       </c>
       <c r="B37">
@@ -10807,7 +10225,7 @@
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="1">
         <v>-35.5</v>
       </c>
       <c r="B38">
@@ -10884,7 +10302,7 @@
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="1">
         <v>-37</v>
       </c>
       <c r="B39">
@@ -10961,7 +10379,7 @@
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="1">
         <v>-38.1</v>
       </c>
       <c r="B40">
@@ -11038,7 +10456,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>-39</v>
       </c>
       <c r="B41">
@@ -11115,7 +10533,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>-40</v>
       </c>
       <c r="B42">
@@ -11192,8 +10610,8 @@
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>-41</v>
+      <c r="A43" s="1">
+        <v>-42</v>
       </c>
       <c r="B43">
         <v>38.40929193717357</v>
@@ -11275,10 +10693,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Y1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11288,76 +10706,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>587.76379147609202</v>
+        <v>769.59517941906802</v>
       </c>
       <c r="C1" s="1">
-        <v>894.53524404475399</v>
+        <v>1095.93721645449</v>
       </c>
       <c r="D1" s="1">
-        <v>1685.9540334445801</v>
+        <v>1847.6450571768901</v>
       </c>
       <c r="E1" s="1">
-        <v>2685.7260619399099</v>
+        <v>2702.4626494673798</v>
       </c>
       <c r="F1" s="1">
-        <v>3496.8083549493899</v>
+        <v>3548.33191101282</v>
       </c>
       <c r="G1" s="1">
-        <v>4364.7422105529904</v>
+        <v>4389.2933019460697</v>
       </c>
       <c r="H1" s="1">
-        <v>5199.3908910112796</v>
+        <v>5231.4400487534604</v>
       </c>
       <c r="I1" s="1">
-        <v>6052.4248793276702</v>
+        <v>6072.9728815016297</v>
       </c>
       <c r="J1" s="1">
-        <v>7156.6485368989897</v>
+        <v>7185.4974858649903</v>
       </c>
       <c r="K1" s="1">
-        <v>7715.98666897149</v>
+        <v>7733.8088536306104</v>
       </c>
       <c r="L1" s="1">
-        <v>8782.8961653280094</v>
+        <v>8809.2383050809494</v>
       </c>
       <c r="M1" s="1">
-        <v>10339.911103843</v>
+        <v>10360.316923390599</v>
       </c>
       <c r="N1" s="1">
-        <v>12283.889776092799</v>
+        <v>12309.539898790201</v>
       </c>
       <c r="O1" s="1">
-        <v>14114.863424078299</v>
+        <v>14139.570367816201</v>
       </c>
       <c r="P1" s="1">
-        <v>15421.436610549301</v>
+        <v>15453.968792120701</v>
       </c>
       <c r="Q1" s="1">
-        <v>18728.348037871299</v>
+        <v>18765.617483101301</v>
       </c>
       <c r="R1" s="1">
-        <v>21441.2179917748</v>
+        <v>21485.3084719656</v>
       </c>
       <c r="S1" s="1">
-        <v>26502.907300478098</v>
+        <v>26564.410371239199</v>
       </c>
       <c r="T1" s="1">
-        <v>31331.188571848899</v>
+        <v>31417.981095376301</v>
       </c>
       <c r="U1" s="1">
-        <v>35824.977101111399</v>
+        <v>35935.318912369003</v>
       </c>
       <c r="V1" s="1">
-        <v>39260.830775698298</v>
+        <v>39394.046467443899</v>
       </c>
       <c r="W1" s="1">
-        <v>42536.195150443797</v>
+        <v>42691.882795442398</v>
       </c>
       <c r="X1" s="1">
-        <v>45465.994903146697</v>
+        <v>45640.202475418002</v>
       </c>
       <c r="Y1" s="1">
-        <v>51612.234836290998</v>
+        <v>51859.980828608699</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -11511,7 +10929,7 @@
         <v>3715148.1882164301</v>
       </c>
       <c r="Y4" s="1">
-        <v>4217373.9109924799</v>
+        <v>4235495.0943433102</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -11588,7 +11006,7 @@
         <v>2978381.29084189</v>
       </c>
       <c r="Y5" s="1">
-        <v>4284449.2636098899</v>
+        <v>4302531.5954806898</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -11665,7 +11083,7 @@
         <v>3064763.5866554789</v>
       </c>
       <c r="Y6" s="1">
-        <v>4421599.4183441196</v>
+        <v>4431703.8613596996</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -11742,7 +11160,7 @@
         <v>3123180.4664046741</v>
       </c>
       <c r="Y7" s="1">
-        <v>4519056.9895853</v>
+        <v>4518146.7430723496</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -11819,7 +11237,7 @@
         <v>3182948.2504570931</v>
       </c>
       <c r="Y8" s="1">
-        <v>4628946.88624423</v>
+        <v>4609100.6883866601</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -11896,7 +11314,7 @@
         <v>3220105.299457869</v>
       </c>
       <c r="Y9" s="1">
-        <v>4696886.1091856798</v>
+        <v>4665281.3549855398</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -11973,7 +11391,7 @@
         <v>3260346.417348817</v>
       </c>
       <c r="Y10" s="1">
-        <v>4776059.0270261997</v>
+        <v>4726903.4452141803</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -12050,7 +11468,7 @@
         <v>3282084.282365812</v>
       </c>
       <c r="Y11" s="1">
-        <v>4846194.9861611901</v>
+        <v>4771821.4116742099</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -12127,7 +11545,7 @@
         <v>3296197.044618112</v>
       </c>
       <c r="Y12" s="1">
-        <v>4905120.4762008404</v>
+        <v>4802094.1402403703</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -12204,7 +11622,7 @@
         <v>3298761.361426814</v>
       </c>
       <c r="Y13" s="1">
-        <v>4951334.1403214801</v>
+        <v>4816792.1221114304</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -12281,7 +11699,7 @@
         <v>3286451.8342421632</v>
       </c>
       <c r="Y14" s="1">
-        <v>4982005.5781040499</v>
+        <v>4806109.4324945798</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -12358,7 +11776,7 @@
         <v>3263184.1038820529</v>
       </c>
       <c r="Y15" s="1">
-        <v>4994468.5386776701</v>
+        <v>4774892.8022672301</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -12435,7 +11853,7 @@
         <v>3230528.9217153592</v>
       </c>
       <c r="Y16" s="1">
-        <v>4987046.6483135698</v>
+        <v>4723250.45555415</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -12512,7 +11930,7 @@
         <v>3192447.0275716032</v>
       </c>
       <c r="Y17" s="1">
-        <v>4962310.0705819</v>
+        <v>4659603.6737921899</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -12589,7 +12007,7 @@
         <v>3139101.2432379681</v>
       </c>
       <c r="Y18" s="1">
-        <v>4910076.7461911803</v>
+        <v>4580300.7417479204</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -12666,7 +12084,7 @@
         <v>3085148.648842575</v>
       </c>
       <c r="Y19" s="1">
-        <v>4844901.1359844003</v>
+        <v>4493880.68601075</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -12743,7 +12161,7 @@
         <v>3025605.1950352001</v>
       </c>
       <c r="Y20" s="1">
-        <v>4762292.2830301197</v>
+        <v>4393876.3332722997</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -12820,7 +12238,7 @@
         <v>2960341.6990266768</v>
       </c>
       <c r="Y21" s="1">
-        <v>4662094.1879299898</v>
+        <v>4280549.4716282701</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -12897,7 +12315,7 @@
         <v>2889137.7876696959</v>
       </c>
       <c r="Y22" s="1">
-        <v>4544288.5230725901</v>
+        <v>4154232.72484947</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -12974,7 +12392,7 @@
         <v>2812218.1576470118</v>
       </c>
       <c r="Y23" s="1">
-        <v>4408990.8728272496</v>
+        <v>4015330.3491565902</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -13051,7 +12469,7 @@
         <v>2729460.1892098701</v>
       </c>
       <c r="Y24" s="1">
-        <v>4256449.2996079</v>
+        <v>3864320.3109772499</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -13128,7 +12546,7 @@
         <v>2640803.726719093</v>
       </c>
       <c r="Y25" s="1">
-        <v>4087045.3201342402</v>
+        <v>3701758.0153174498</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -13205,7 +12623,7 @@
         <v>2546212.5725611532</v>
       </c>
       <c r="Y26" s="1">
-        <v>3901297.6409672499</v>
+        <v>3528282.2662337301</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -13282,7 +12700,7 @@
         <v>2445952.436945288</v>
       </c>
       <c r="Y27" s="1">
-        <v>3699869.3650770299</v>
+        <v>3344624.4091634098</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -13359,7 +12777,7 @@
         <v>2340005.4315581489</v>
       </c>
       <c r="Y28" s="1">
-        <v>3483579.9670185</v>
+        <v>3151622.2879163302</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -13436,7 +12854,7 @@
         <v>2228353.3406206481</v>
       </c>
       <c r="Y29" s="1">
-        <v>3253386.1207580301</v>
+        <v>2950279.90771541</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -13513,7 +12931,7 @@
         <v>2103975.6932307109</v>
       </c>
       <c r="Y30" s="1">
-        <v>3011313.6971360999</v>
+        <v>2754176.8195004999</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -13590,7 +13008,7 @@
         <v>1966767.6077799781</v>
       </c>
       <c r="Y31" s="1">
-        <v>2758582.54667213</v>
+        <v>2548434.0323502799</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -13667,10 +13085,10 @@
         <v>1739265.4183112041</v>
       </c>
       <c r="Y32" s="1">
-        <v>2359675.5848610601</v>
+        <v>2222280.2424821099</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>-30</v>
       </c>
@@ -13744,10 +13162,10 @@
         <v>1483236.765817299</v>
       </c>
       <c r="Y33" s="1">
-        <v>1945610.4228588899</v>
+        <v>1880350.08042416</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>-31</v>
       </c>
@@ -13821,10 +13239,10 @@
         <v>1305880.291243376</v>
       </c>
       <c r="Y34" s="1">
-        <v>1678145.2904486</v>
+        <v>1655326.2998215</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>-32</v>
       </c>
@@ -13898,10 +13316,10 @@
         <v>1127119.835093955</v>
       </c>
       <c r="Y35" s="1">
-        <v>1423479.1098921499</v>
+        <v>1439695.9809106099</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>-33</v>
       </c>
@@ -13975,10 +13393,10 @@
         <v>950922.30338995624</v>
       </c>
       <c r="Y36" s="1">
-        <v>1183807.7017788701</v>
+        <v>1236072.69115966</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>-34</v>
       </c>
@@ -14052,10 +13470,10 @@
         <v>783116.62616362434</v>
       </c>
       <c r="Y37" s="1">
-        <v>960857.68070996902</v>
+        <v>1046432.2915539501</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>-35.5</v>
       </c>
@@ -14129,10 +13547,10 @@
         <v>554614.24292993627</v>
       </c>
       <c r="Y38" s="1">
-        <v>661055.73924759496</v>
+        <v>791654.05305870902</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>-37</v>
       </c>
@@ -14206,10 +13624,10 @@
         <v>363918.11386950081</v>
       </c>
       <c r="Y39" s="1">
-        <v>406902.151588879</v>
+        <v>577549.35503062897</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>-38.1</v>
       </c>
@@ -14283,10 +13701,10 @@
         <v>253958.11433268359</v>
       </c>
       <c r="Y40" s="1">
-        <v>251523.46016816</v>
+        <v>448457.15194733901</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>-39</v>
       </c>
@@ -14360,10 +13778,10 @@
         <v>177242.60492635251</v>
       </c>
       <c r="Y41" s="1">
-        <v>149023.05007300799</v>
+        <v>329597.57901366398</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>-40</v>
       </c>
@@ -14437,12 +13855,12 @@
         <v>106804.5159387101</v>
       </c>
       <c r="Y42" s="1">
-        <v>64601.459795608498</v>
+        <v>214205.782486921</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>-41.9</v>
+        <v>-42</v>
       </c>
       <c r="B43">
         <v>62.638336514607772</v>
@@ -14514,9 +13932,8 @@
         <v>42916.521256319931</v>
       </c>
       <c r="Y43" s="1">
-        <v>1.3596007103389799E-7</v>
-      </c>
-      <c r="Z43" s="2"/>
+        <v>41084.886777708198</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14529,7 +13946,7 @@
   <dimension ref="A1:Y43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14539,76 +13956,76 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>587.76379147609202</v>
+        <v>769.59517941906802</v>
       </c>
       <c r="C1" s="1">
-        <v>894.53524404475399</v>
+        <v>1095.93721645449</v>
       </c>
       <c r="D1" s="1">
-        <v>1685.9540334445801</v>
+        <v>1847.6450571768901</v>
       </c>
       <c r="E1" s="1">
-        <v>2685.7260619399099</v>
+        <v>2702.4626494673798</v>
       </c>
       <c r="F1" s="1">
-        <v>3496.8083549493899</v>
+        <v>3548.33191101282</v>
       </c>
       <c r="G1" s="1">
-        <v>4364.7422105529904</v>
+        <v>4389.2933019460697</v>
       </c>
       <c r="H1" s="1">
-        <v>5199.3908910112796</v>
+        <v>5231.4400487534604</v>
       </c>
       <c r="I1" s="1">
-        <v>6052.4248793276702</v>
+        <v>6072.9728815016297</v>
       </c>
       <c r="J1" s="1">
-        <v>7156.6485368989897</v>
+        <v>7185.4974858649903</v>
       </c>
       <c r="K1" s="1">
-        <v>7715.98666897149</v>
+        <v>7733.8088536306104</v>
       </c>
       <c r="L1" s="1">
-        <v>8782.8961653280094</v>
+        <v>8809.2383050809494</v>
       </c>
       <c r="M1" s="1">
-        <v>10339.911103843</v>
+        <v>10360.316923390599</v>
       </c>
       <c r="N1" s="1">
-        <v>12283.889776092799</v>
+        <v>12309.539898790201</v>
       </c>
       <c r="O1" s="1">
-        <v>14114.863424078299</v>
+        <v>14139.570367816201</v>
       </c>
       <c r="P1" s="1">
-        <v>15421.436610549301</v>
+        <v>15453.968792120701</v>
       </c>
       <c r="Q1" s="1">
-        <v>18728.348037871299</v>
+        <v>18765.617483101301</v>
       </c>
       <c r="R1" s="1">
-        <v>21441.2179917748</v>
+        <v>21485.3084719656</v>
       </c>
       <c r="S1" s="1">
-        <v>26502.907300478098</v>
+        <v>26564.410371239199</v>
       </c>
       <c r="T1" s="1">
-        <v>31331.188571848899</v>
+        <v>31417.981095376301</v>
       </c>
       <c r="U1" s="1">
-        <v>35824.977101111399</v>
+        <v>35935.318912369003</v>
       </c>
       <c r="V1" s="1">
-        <v>39260.830775698298</v>
+        <v>39394.046467443899</v>
       </c>
       <c r="W1" s="1">
-        <v>42536.195150443797</v>
+        <v>42691.882795442398</v>
       </c>
       <c r="X1" s="1">
-        <v>45465.994903146697</v>
+        <v>45640.202475418002</v>
       </c>
       <c r="Y1" s="1">
-        <v>51612.234836290998</v>
+        <v>51859.980828608699</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -14762,7 +14179,7 @@
         <v>0.70509999999999995</v>
       </c>
       <c r="Y4" s="1">
-        <v>0.97</v>
+        <v>0.97137878821043999</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14839,7 +14256,7 @@
         <v>0.68433415889740046</v>
       </c>
       <c r="Y5" s="1">
-        <v>0.94073927832429804</v>
+        <v>0.94225836884681102</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -14916,7 +14333,7 @@
         <v>0.64271533489227273</v>
       </c>
       <c r="Y6" s="1">
-        <v>0.88135446667655803</v>
+        <v>0.88281559108219199</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -14993,7 +14410,7 @@
         <v>0.61267191171646151</v>
       </c>
       <c r="Y7" s="1">
-        <v>0.83829454250995294</v>
+        <v>0.83970298389717202</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -15070,7 +14487,7 @@
         <v>0.57696545124053933</v>
       </c>
       <c r="Y8" s="1">
-        <v>0.78766515902544598</v>
+        <v>0.78903594666788202</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -15147,7 +14564,7 @@
         <v>0.55386358499526989</v>
       </c>
       <c r="Y9" s="1">
-        <v>0.75456720487645301</v>
+        <v>0.75590383794708604</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -15224,7 +14641,7 @@
         <v>0.52614724636077892</v>
       </c>
       <c r="Y10" s="1">
-        <v>0.71391665141795002</v>
+        <v>0.71522760791612905</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -15301,7 +14718,7 @@
         <v>0.49904212355613692</v>
       </c>
       <c r="Y11" s="1">
-        <v>0.67419039778418799</v>
+        <v>0.67547279103295099</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -15378,7 +14795,7 @@
         <v>0.47291433811187772</v>
       </c>
       <c r="Y12" s="1">
-        <v>0.63536301298841302</v>
+        <v>0.63662037055786103</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -15455,7 +14872,7 @@
         <v>0.44789502024650568</v>
       </c>
       <c r="Y13" s="1">
-        <v>0.59744788705166096</v>
+        <v>0.59868381165102602</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -15532,7 +14949,7 @@
         <v>0.42370122671127358</v>
       </c>
       <c r="Y14" s="1">
-        <v>0.56054153920421901</v>
+        <v>0.56175781540432501</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -15609,7 +15026,7 @@
         <v>0.40009230375289873</v>
       </c>
       <c r="Y15" s="1">
-        <v>0.52459239970265004</v>
+        <v>0.52579293131129301</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -15686,7 +15103,7 @@
         <v>0.37712386250495927</v>
       </c>
       <c r="Y16" s="1">
-        <v>0.48959432276173498</v>
+        <v>0.49078310014256099</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -15763,7 +15180,7 @@
         <v>0.35741215944290139</v>
       </c>
       <c r="Y17" s="1">
-        <v>0.45888368651975298</v>
+        <v>0.46007268871467599</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -15840,7 +15257,7 @@
         <v>0.33362227678298928</v>
       </c>
       <c r="Y18" s="1">
-        <v>0.42221758354362099</v>
+        <v>0.42339478756267102</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -15917,7 +15334,7 @@
         <v>0.31204530596733049</v>
       </c>
       <c r="Y19" s="1">
-        <v>0.38977176282044201</v>
+        <v>0.39094909728395</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -15994,7 +15411,7 @@
         <v>0.29116508364677451</v>
       </c>
       <c r="Y20" s="1">
-        <v>0.35816871814615298</v>
+        <v>0.35935094724759797</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -16071,7 +15488,7 @@
         <v>0.27080154418945329</v>
       </c>
       <c r="Y21" s="1">
-        <v>0.32738993751137402</v>
+        <v>0.32858186557054098</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -16148,7 +15565,7 @@
         <v>0.25092294812202443</v>
       </c>
       <c r="Y22" s="1">
-        <v>0.29741413600727401</v>
+        <v>0.29862059483989201</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -16225,7 +15642,7 @@
         <v>0.2314621508121491</v>
       </c>
       <c r="Y23" s="1">
-        <v>0.26821730144302602</v>
+        <v>0.26944313833681299</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -16302,7 +15719,7 @@
         <v>0.21224410831928239</v>
       </c>
       <c r="Y24" s="1">
-        <v>0.23977273954965</v>
+        <v>0.241022806027475</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -16379,7 +15796,7 @@
         <v>0.19323858618736231</v>
       </c>
       <c r="Y25" s="1">
-        <v>0.21205111565814799</v>
+        <v>0.213330257275611</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -16456,7 +15873,7 @@
         <v>0.17441277205944031</v>
       </c>
       <c r="Y26" s="1">
-        <v>0.18502048802422999</v>
+        <v>0.18633353556508001</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -16533,7 +15950,7 @@
         <v>0.1557512879371642</v>
       </c>
       <c r="Y27" s="1">
-        <v>0.15864632487983199</v>
+        <v>0.15999808752458899</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
@@ -16610,7 +16027,7 @@
         <v>0.13722765445709231</v>
       </c>
       <c r="Y28" s="1">
-        <v>0.132891491385599</v>
+        <v>0.13428675283887301</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
@@ -16687,7 +16104,7 @@
         <v>0.1189173907041552</v>
       </c>
       <c r="Y29" s="1">
-        <v>0.10771618046411199</v>
+        <v>0.109159699886867</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
@@ -16764,7 +16181,7 @@
         <v>0.10069510340690629</v>
       </c>
       <c r="Y30" s="1">
-        <v>8.29736055565133E-2</v>
+        <v>8.4463989575823503E-2</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
@@ -16841,7 +16258,7 @@
         <v>8.244449645280838E-2</v>
       </c>
       <c r="Y31" s="1">
-        <v>5.8757636784181298E-2</v>
+        <v>6.0299702101401301E-2</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -16918,7 +16335,7 @@
         <v>5.4843995720148107E-2</v>
       </c>
       <c r="Y32" s="1">
-        <v>2.33425078470871E-2</v>
+        <v>2.4973141860952099E-2</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.25">
@@ -16995,7 +16412,7 @@
         <v>2.7676869183778759E-2</v>
       </c>
       <c r="Y33" s="1">
-        <v>-1.11403354297211E-2</v>
+        <v>-9.4079675965762308E-3</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.25">
@@ -17072,7 +16489,7 @@
         <v>9.3482779338955827E-3</v>
       </c>
       <c r="Y34" s="1">
-        <v>-3.3780880624724299E-2</v>
+        <v>-3.1968653732251398E-2</v>
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.25">
@@ -17149,7 +16566,7 @@
         <v>-8.864600211381914E-3</v>
       </c>
       <c r="Y35" s="1">
-        <v>-5.6247345389732702E-2</v>
+        <v>-5.4349178650244599E-2</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.25">
@@ -17226,7 +16643,7 @@
         <v>-2.7006683871150041E-2</v>
       </c>
       <c r="Y36" s="1">
-        <v>-7.8597189355710806E-2</v>
+        <v>-7.66082553770535E-2</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.25">
@@ -17303,7 +16720,7 @@
         <v>-4.5374345034360837E-2</v>
       </c>
       <c r="Y37" s="1">
-        <v>-0.100880590735083</v>
+        <v>-9.8796770034495898E-2</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.25">
@@ -17380,7 +16797,7 @@
         <v>-7.3365755379200009E-2</v>
       </c>
       <c r="Y38" s="1">
-        <v>-0.1342794233274</v>
+        <v>-0.13204635856904601</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.25">
@@ -17457,7 +16874,7 @@
         <v>-0.1017827391624451</v>
       </c>
       <c r="Y39" s="1">
-        <v>-0.16776725085724301</v>
+        <v>-0.16537917004389599</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.25">
@@ -17534,7 +16951,7 @@
         <v>-0.1237360537052154</v>
       </c>
       <c r="Y40" s="1">
-        <v>-0.192448809280408</v>
+        <v>-0.18994441555804401</v>
       </c>
     </row>
     <row r="41" spans="1:25" x14ac:dyDescent="0.25">
@@ -17611,7 +17028,7 @@
         <v>-0.14209932088851909</v>
       </c>
       <c r="Y41" s="1">
-        <v>-0.21245768606427701</v>
+        <v>-0.20985740725969901</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.25">
@@ -17688,12 +17105,12 @@
         <v>-0.16181510686874409</v>
       </c>
       <c r="Y42" s="1">
-        <v>-0.23479488980530799</v>
+        <v>-0.232086793753283</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>-41.9</v>
+        <v>-42</v>
       </c>
       <c r="B43">
         <v>-1.2708277790807179E-4</v>
@@ -17765,7 +17182,7 @@
         <v>-0.1810180544853208</v>
       </c>
       <c r="Y43" s="1">
-        <v>-0.27765554575005102</v>
+        <v>-0.27699562167408698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>